<commit_message>
Finished refreshment-script for BGY16.
</commit_message>
<xml_diff>
--- a/_HBF IT 17/Daten/BevDE.xlsx
+++ b/_HBF IT 17/Daten/BevDE.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carso\Documents\bbs1\HBF IT\Daten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carso\Documents\bbs1\_HBF IT 17\Daten\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B002AD-D6A2-4EBF-B9E0-F5FFCAA002F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,6 +377,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -394,9 +398,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,6 +510,51 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>'12411-0001'!$A$6:$A$72</c:f>
@@ -2049,39 +2095,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1">
@@ -2089,7 +2135,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1">
@@ -2097,7 +2143,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1">
@@ -2105,7 +2151,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1">
@@ -2113,7 +2159,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="1">
@@ -2121,7 +2167,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="1">
@@ -2129,7 +2175,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="1">
@@ -2137,7 +2183,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="1">
@@ -2145,7 +2191,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="1">
@@ -2153,7 +2199,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="1">
@@ -2161,7 +2207,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="1">
@@ -2169,7 +2215,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1">
@@ -2177,7 +2223,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="1">
@@ -2185,7 +2231,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="1">
@@ -2193,7 +2239,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="1">
@@ -2201,7 +2247,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="1">
@@ -2209,7 +2255,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="1">
@@ -2217,7 +2263,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="1">
@@ -2225,7 +2271,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="1">
@@ -2233,7 +2279,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="1">
@@ -2241,7 +2287,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="1">
@@ -2249,7 +2295,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="1">
@@ -2257,7 +2303,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="1">
@@ -2265,7 +2311,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="1">
@@ -2273,7 +2319,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="1">
@@ -2281,7 +2327,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="1">
@@ -2289,7 +2335,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="1">
@@ -2297,7 +2343,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="1">
@@ -2305,7 +2351,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="1">
@@ -2313,7 +2359,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="1">
@@ -2321,7 +2367,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="1">
@@ -2329,7 +2375,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="1">
@@ -2337,7 +2383,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="1">
@@ -2345,7 +2391,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="1">
@@ -2353,7 +2399,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="1">
@@ -2361,7 +2407,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="1">
@@ -2369,7 +2415,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="1">
@@ -2377,7 +2423,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="1">
@@ -2385,7 +2431,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="1">
@@ -2393,7 +2439,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="1">
@@ -2401,7 +2447,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="1">
@@ -2409,7 +2455,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="1">
@@ -2417,7 +2463,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="1">
@@ -2425,7 +2471,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="1">
@@ -2433,7 +2479,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="1">
@@ -2441,7 +2487,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="1">
@@ -2449,7 +2495,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="1">
@@ -2457,7 +2503,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="1">
@@ -2465,7 +2511,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="1">
@@ -2473,7 +2519,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="1">
@@ -2481,7 +2527,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="1">
@@ -2489,7 +2535,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="1">
@@ -2497,7 +2543,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="1">
@@ -2505,7 +2551,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B59" s="1">
@@ -2513,7 +2559,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="1">
@@ -2521,7 +2567,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="1">
@@ -2529,7 +2575,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B62" s="1">
@@ -2537,7 +2583,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B63" s="1">
@@ -2545,7 +2591,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B64" s="1">
@@ -2553,7 +2599,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B65" s="1">
@@ -2561,7 +2607,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B66" s="1">
@@ -2569,7 +2615,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B67" s="1">
@@ -2577,7 +2623,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B68" s="1">
@@ -2585,7 +2631,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="1">
@@ -2593,7 +2639,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="1">
@@ -2601,7 +2647,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="1">
@@ -2609,7 +2655,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B72" s="1">

</xml_diff>